<commit_message>
correccion en los jframes de luis
</commit_message>
<xml_diff>
--- a/rom/Bills/BillSale.xlsx
+++ b/rom/Bills/BillSale.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,120 @@
   </si>
   <si>
     <t>PL18</t>
+  </si>
+  <si>
+    <t>BS44</t>
+  </si>
+  <si>
+    <t>jhon</t>
+  </si>
+  <si>
+    <t>BS45</t>
+  </si>
+  <si>
+    <t>BS46</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>Balazos</t>
+  </si>
+  <si>
+    <t>PL19</t>
+  </si>
+  <si>
+    <t>BS47</t>
+  </si>
+  <si>
+    <t>BS48</t>
+  </si>
+  <si>
+    <t>BS49</t>
+  </si>
+  <si>
+    <t>ggg</t>
+  </si>
+  <si>
+    <t>BS50</t>
+  </si>
+  <si>
+    <t>jjjj</t>
+  </si>
+  <si>
+    <t>BS51</t>
+  </si>
+  <si>
+    <t>jjhfjh</t>
+  </si>
+  <si>
+    <t>BS52</t>
+  </si>
+  <si>
+    <t>dffff</t>
+  </si>
+  <si>
+    <t>BS53</t>
+  </si>
+  <si>
+    <t>mnhhh</t>
+  </si>
+  <si>
+    <t>BS54</t>
+  </si>
+  <si>
+    <t>nhn</t>
+  </si>
+  <si>
+    <t>BS55</t>
+  </si>
+  <si>
+    <t>jjh</t>
+  </si>
+  <si>
+    <t>BS56</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>BS57</t>
+  </si>
+  <si>
+    <t>BS58</t>
+  </si>
+  <si>
+    <t>BS59</t>
+  </si>
+  <si>
+    <t>111111</t>
+  </si>
+  <si>
+    <t>BS60</t>
+  </si>
+  <si>
+    <t>jhhon</t>
+  </si>
+  <si>
+    <t>BS61</t>
+  </si>
+  <si>
+    <t>kdkkd</t>
+  </si>
+  <si>
+    <t>BS62</t>
+  </si>
+  <si>
+    <t>BS63</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>BS64</t>
+  </si>
+  <si>
+    <t>jsjs</t>
   </si>
 </sst>
 </file>
@@ -110,7 +224,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -179,7 +293,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C3" t="n">
         <v>2250.0</v>
@@ -194,13 +308,129 @@
         <v>2250.0</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2250.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2250.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20200.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20191.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2250.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2241.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="n">
+        <v>20200.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>20200.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>